<commit_message>
update re-registration templete file
</commit_message>
<xml_diff>
--- a/webdata/ReRegistrationExcel.xlsx
+++ b/webdata/ReRegistrationExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0208058/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/B0208058/Documents/slretailer-web-portal/webdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68CC5BD-1073-B74A-ADD7-2D2C76B77C0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2B4568-5254-8447-92BE-C0D614B623DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{AD25A3D4-5914-714C-9B57-13C12854785D}"/>
   </bookViews>
@@ -390,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2559CB3C-E1FB-7F4C-BD8B-350E92BA430D}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -402,7 +402,7 @@
     <col min="2" max="2" width="39.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +410,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6"/>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16"/>
+      <c r="C16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>